<commit_message>
se agrego el archivo de distribucion de trabajo
</commit_message>
<xml_diff>
--- a/Documentacion/Distribución de Trabajo (TI).xlsx
+++ b/Documentacion/Distribución de Trabajo (TI).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-20\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE618DC9-E394-4D1E-B8F0-AFF44EB5884F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854EC291-92E9-40AB-A6F9-C47ABDB020D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AB28C158-560D-4BBB-BC35-7D89BF765275}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB28C158-560D-4BBB-BC35-7D89BF765275}"/>
   </bookViews>
   <sheets>
     <sheet name="Proyecto Hospital - 7A" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="118">
   <si>
     <t>Num.</t>
   </si>
@@ -2472,6 +2472,9 @@
 19.	Disponibilidad de recursos pediátricos: Se debe garantizar la disponibilidad de equipos médicos, medicamentos y otros recursos necesarios para la atención adecuada de pacientes pediátricos, asegurando su mantenimiento y reposición oportuna.
 20.	Comunicación con el paciente y la familia: Se debe fomentar una comunicación abierta y transparente con los pacientes pediátricos y sus familias, proporcionando información clara sobre su diagnóstico, tratamiento y pronóstico, adaptada a su nivel de comprensión y edad.
 </t>
+  </si>
+  <si>
+    <t>pacientes</t>
   </si>
 </sst>
 </file>
@@ -3069,28 +3072,28 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H6" sqref="H6"/>
+      <selection pane="topRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.21875" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="58" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" customWidth="1"/>
-    <col min="6" max="6" width="45.109375" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
     <col min="9" max="9" width="42" customWidth="1"/>
-    <col min="10" max="10" width="37.21875" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="307.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="307.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -3146,7 +3149,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -3170,7 +3173,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -3198,9 +3201,11 @@
       <c r="I7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="J7" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -3224,7 +3229,7 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -3246,7 +3251,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="215.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -3270,7 +3275,7 @@
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -3294,7 +3299,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -3316,7 +3321,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -3342,7 +3347,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3354,7 +3359,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3368,7 +3373,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3380,7 +3385,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3394,7 +3399,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3406,7 +3411,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3420,7 +3425,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3432,7 +3437,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3446,7 +3451,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3458,7 +3463,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3472,7 +3477,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3484,7 +3489,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3498,7 +3503,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3510,7 +3515,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3524,7 +3529,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3536,7 +3541,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3550,7 +3555,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3562,7 +3567,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3576,7 +3581,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3588,7 +3593,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3602,7 +3607,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3614,7 +3619,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3628,7 +3633,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3640,7 +3645,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3654,7 +3659,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3666,7 +3671,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -3680,7 +3685,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3692,7 +3697,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3706,7 +3711,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3718,7 +3723,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3732,7 +3737,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3744,7 +3749,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3758,7 +3763,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3788,28 +3793,28 @@
       <selection pane="topRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.21875" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="58" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" customWidth="1"/>
-    <col min="6" max="6" width="41.77734375" customWidth="1"/>
-    <col min="7" max="7" width="48.77734375" customWidth="1"/>
-    <col min="8" max="8" width="34.33203125" customWidth="1"/>
-    <col min="9" max="9" width="32.109375" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" customWidth="1"/>
+    <col min="7" max="7" width="48.7109375" customWidth="1"/>
+    <col min="8" max="8" width="34.28515625" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" customWidth="1"/>
-    <col min="14" max="14" width="50.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -3844,7 +3849,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -3867,7 +3872,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="268.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="268.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -3895,7 +3900,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="270" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -3925,7 +3930,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="281.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="281.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -3953,7 +3958,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="279.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="279.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -3978,7 +3983,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="168" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -4005,7 +4010,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="270" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -4030,7 +4035,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="266.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="266.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -4055,7 +4060,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4068,7 +4073,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4081,7 +4086,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>

</xml_diff>